<commit_message>
file standardised for VIP and temp DB both and new config file updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishGulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC9816F-9C2B-44B5-85C9-444BD57DB44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75316D56-2F93-4646-8869-DBDE99147B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
-    <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Settingsold" sheetId="1" r:id="rId1"/>
+    <sheet name="Settings" sheetId="4" r:id="rId2"/>
+    <sheet name="Constants" sheetId="2" r:id="rId3"/>
+    <sheet name="Assets" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -117,24 +118,15 @@
     <t>InputPartnerFilePath</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/No Socios</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/Socios</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/No Socios</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/Socios</t>
   </si>
   <si>
     <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos</t>
-  </si>
-  <si>
     <t>input file path for partner file</t>
   </si>
   <si>
@@ -147,17 +139,77 @@
     <t>SOCIOS_BD_Argentina_Semana_Sema</t>
   </si>
   <si>
-    <t>VIPfilePath</t>
-  </si>
-  <si>
-    <t>VIPSheetName</t>
+    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos</t>
+  </si>
+  <si>
+    <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /Planeacion/0.Envios TS 2021/0 Envios 0/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>SurvayFileTraditionalPath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>BDVIPfilePath</t>
+  </si>
+  <si>
+    <t>BDVIPSheetName</t>
+  </si>
+  <si>
+    <t>InputSheetName</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>InputSheetNewName</t>
+  </si>
+  <si>
+    <t>InputVIPSheetName</t>
+  </si>
+  <si>
+    <t>LUXURY</t>
+  </si>
+  <si>
+    <t>TRADICIONAL</t>
+  </si>
+  <si>
+    <t>BDTempFilePath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>BDTempSheetName</t>
+  </si>
+  <si>
+    <t>SurveyTradFilePath</t>
+  </si>
+  <si>
+    <t>SurveyTradSheetName</t>
+  </si>
+  <si>
+    <t>SurveyVipFilePath</t>
+  </si>
+  <si>
+    <t>SurveyVipSheetName</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/VIP</t>
+  </si>
+  <si>
+    <t>BD_ENCUESTA_LARGA_GULF_VIP_Sema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -262,16 +314,22 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,10 +374,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,19 +386,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,16 +716,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="68" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -678,7 +734,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -712,7 +768,7 @@
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="2"/>
@@ -721,15 +777,15 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>17</v>
+      <c r="B3" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="4"/>
@@ -738,40 +794,40 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>36</v>
+      <c r="B5" s="25" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>34</v>
+      <c r="B6" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>33</v>
+      <c r="B7" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>35</v>
+      <c r="B8" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>36</v>
+      <c r="B9" s="25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -779,21 +835,21 @@
         <v>30</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>31</v>
+      <c r="B11" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -808,7 +864,7 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="23" t="s">
         <v>19</v>
       </c>
     </row>
@@ -816,7 +872,7 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="24" t="s">
         <v>20</v>
       </c>
     </row>
@@ -824,46 +880,49 @@
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="24" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
+      <c r="B19" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1827,7 +1886,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1839,6 +1897,190 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="25"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
@@ -2902,7 +3144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>

</xml_diff>

<commit_message>
gulf portal changes for no VIP file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisGulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DEB48-F024-49FD-AA5A-3F304D9E9EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B77A65-889E-460D-A7B0-39D9D2F27B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="0" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settingsold" sheetId="1" r:id="rId1"/>
-    <sheet name="Settings" sheetId="4" r:id="rId2"/>
-    <sheet name="Constants" sheetId="2" r:id="rId3"/>
-    <sheet name="Assets" sheetId="3" r:id="rId4"/>
+    <sheet name="Settings" sheetId="4" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -49,15 +48,9 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>DirectorioClavesPath</t>
-  </si>
-  <si>
     <t>BlackListTrackingPath</t>
   </si>
   <si>
-    <t>TRADPath</t>
-  </si>
-  <si>
     <t>FTPport</t>
   </si>
   <si>
@@ -73,9 +66,6 @@
     <t>in_BlackListSheetName</t>
   </si>
   <si>
-    <t>in_TradSheetName</t>
-  </si>
-  <si>
     <t>Hoja 1</t>
   </si>
   <si>
@@ -88,72 +78,24 @@
     <t>rpanotificaciones@tecnoyar.com</t>
   </si>
   <si>
-    <t>TempSheetName</t>
-  </si>
-  <si>
     <t>GmailID</t>
   </si>
   <si>
     <t>GmailPass</t>
   </si>
   <si>
-    <t>NO_SOCIOS_BD_Argentina__Semana_</t>
-  </si>
-  <si>
     <t>notificacionesrpa.tecnoyar@gmail.com</t>
   </si>
   <si>
     <t>Rp4.C1n3p0l1s</t>
   </si>
   <si>
-    <t>PartnerTempBDPath</t>
-  </si>
-  <si>
-    <t>NonPartnerTempBDPath</t>
-  </si>
-  <si>
     <t>InputnonPartnerFilePath</t>
   </si>
   <si>
-    <t>InputPartnerFilePath</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/Socios</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/Socios</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
-  </si>
-  <si>
-    <t>input file path for partner file</t>
-  </si>
-  <si>
-    <t>input file path for non partner file</t>
-  </si>
-  <si>
-    <t>TempPartnerSheetName</t>
-  </si>
-  <si>
-    <t>SOCIOS_BD_Argentina_Semana_Sema</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos</t>
-  </si>
-  <si>
     <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
   </si>
   <si>
-    <t xml:space="preserve"> /Planeacion/0.Envios TS 2021/0 Envios 0/GULF/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>SurvayFileTraditionalPath</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>BDVIPfilePath</t>
   </si>
   <si>
@@ -199,9 +141,6 @@
     <t>BD_ENCUESTA_LARGA_GULF_VIP_Sema</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/GULF/Base de Datos</t>
-  </si>
-  <si>
     <t>Nombre de la hoja VIP en excel</t>
   </si>
   <si>
@@ -220,18 +159,12 @@
     <t>Nombre de hoja blacklist</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/GULF/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>Ruta de BD Tradicional exportada</t>
   </si>
   <si>
     <t>Ruta de BD VIP exportada</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/GULF/VIP</t>
-  </si>
-  <si>
     <t>Ruta de archivo template Tradicional</t>
   </si>
   <si>
@@ -244,7 +177,16 @@
     <t>Nombre de la hoja del archivo Template Tradicional</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/GULF/TRADICIONAL</t>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -388,14 +330,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -417,15 +356,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -748,18 +678,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="72" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -767,7 +914,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -797,1405 +944,6 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{FF7F0B36-CE90-4A91-B3A6-3587652CB510}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
-      <c r="A4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z978"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
@@ -2209,29 +957,29 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B5" s="14"/>
+      <c r="B5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3210,7 +1958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
@@ -3272,17 +2020,17 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="10"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -3292,22 +2040,22 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
testing of bot done.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisGulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B77A65-889E-460D-A7B0-39D9D2F27B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C84B750-7689-4F0B-9C02-EAD37854FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="0" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -177,23 +177,130 @@
     <t>Nombre de la hoja del archivo Template Tradicional</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/GULF/Base de Datos/Exportadas</t>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>CorrectSheetName</t>
+  </si>
+  <si>
+    <t>WorkingStartDate</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>WorkingEndDate</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- Data doesn't belong to this week</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailBody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+Please find the below data which does not belong to current week.&lt;br/&gt;
+[Nothisweekdatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>MailTo</t>
+  </si>
+  <si>
+    <t>rhernandez@tecnoyar.com.mx</t>
+  </si>
+  <si>
+    <t>MailCC</t>
+  </si>
+  <si>
+    <t>arerodriguez@tecnoyar.com</t>
+  </si>
+  <si>
+    <t>InputFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Error- Input file Notification</t>
+  </si>
+  <si>
+    <t>InputFileExceptionbody</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Notification- Not All file Got downloaded</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionbody</t>
+  </si>
+  <si>
+    <t>WrongNameMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- name is not correct</t>
+  </si>
+  <si>
+    <t>WrongNameMailbody</t>
+  </si>
+  <si>
+    <t>NADirectrioMailSubject</t>
+  </si>
+  <si>
+    <t>file of the Maxico mark contains errors in the "N" column called "clave_tipo_cine"</t>
+  </si>
+  <si>
+    <t>NADirectrioMailBody</t>
+  </si>
+  <si>
+    <t>#NA data found at input file in "N" column</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepolish Gulf run, below is the detail of error&lt;br/&gt;
+[error]&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepos Gulf process run, below is the detail of error&lt;br/&gt;
+Not all required files got downloaded from FTP&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+below names are not correct in Gulf process input file.&lt;br/&gt;
+[wrongnamedatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,6 +311,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -287,12 +395,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -330,13 +432,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -347,9 +446,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -364,7 +461,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,23 +790,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -706,7 +817,7 @@
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C2" t="s">
@@ -728,7 +839,7 @@
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
@@ -739,7 +850,7 @@
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
@@ -748,14 +859,14 @@
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="2"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>52</v>
+      <c r="B7" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -777,7 +888,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -798,7 +909,7 @@
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C12" t="s">
@@ -809,7 +920,7 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
@@ -820,7 +931,7 @@
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C15" t="s">
@@ -839,7 +950,7 @@
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C18" t="s">
@@ -858,7 +969,7 @@
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="13">
         <v>21</v>
       </c>
     </row>
@@ -866,7 +977,7 @@
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -874,16 +985,26 @@
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -898,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -945,66 +1066,206 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="19">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="24" t="s">
         <v>20</v>
       </c>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="24" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B5" s="13"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="19"/>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="2"/>
+      <c r="A7" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="19"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="19"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="19"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="19"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="20">
+        <v>44599</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="20">
+        <v>44605</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2020,17 +2281,17 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -2040,22 +2301,22 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="14"/>
+      <c r="B21" s="12"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
process updated for blacklist vip
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisGulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C84B750-7689-4F0B-9C02-EAD37854FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016F2CE2-D3DD-42DC-AFCD-AA5F49AF091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -175,18 +175,6 @@
   </si>
   <si>
     <t>Nombre de la hoja del archivo Template Tradicional</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/GULF/Base de Datos/Exportadas</t>
   </si>
   <si>
     <t>CorrectnameFilePath</t>
@@ -295,12 +283,27 @@
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>Black list</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -411,6 +414,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -432,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -476,6 +486,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,7 +829,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -866,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -888,7 +899,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -910,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
@@ -921,7 +932,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -932,7 +943,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -951,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>46</v>
@@ -999,19 +1010,21 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>56</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B28" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1019,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1101,19 +1114,19 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" s="19"/>
     </row>
@@ -1124,19 +1137,19 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C10" s="19"/>
     </row>
@@ -1147,19 +1160,19 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" s="19"/>
     </row>
@@ -1170,19 +1183,19 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C16" s="19"/>
     </row>
@@ -1193,19 +1206,19 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C19" s="19"/>
     </row>
@@ -1216,19 +1229,19 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C22" s="19"/>
     </row>
@@ -1239,24 +1252,24 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B24" s="20">
-        <v>44599</v>
+        <v>44606</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B25" s="20">
-        <v>44605</v>
+        <v>44612</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
rename blacklist and input files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisGulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016F2CE2-D3DD-42DC-AFCD-AA5F49AF091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998EB887-CBDF-467A-BD70-2DF7378F9D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,19 +284,19 @@
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/08 Envío Semana 08/GULF/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>Black list</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/GULF/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/GULF/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/GULF/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/GULF/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -829,7 +829,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -877,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -899,7 +899,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -921,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
@@ -932,7 +932,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -943,7 +943,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -962,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
         <v>46</v>
@@ -1255,7 +1255,7 @@
         <v>53</v>
       </c>
       <c r="B24" s="20">
-        <v>44606</v>
+        <v>44613</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>54</v>
@@ -1266,7 +1266,7 @@
         <v>55</v>
       </c>
       <c r="B25" s="20">
-        <v>44612</v>
+        <v>44619</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>54</v>

</xml_diff>